<commit_message>
Added list of Russian segment modules
</commit_message>
<xml_diff>
--- a/docs/ISS Mimic Magnet Mapping.xlsx
+++ b/docs/ISS Mimic Magnet Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pferr\Desktop\ISS Mimic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAFB51E4-58F8-42D8-BFBC-269326CEAC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C377F575-29D0-408B-B976-DA73AED5014E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D443E188-A2A4-49B6-9865-B6F9C3BED1B3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="56">
   <si>
     <t>Module Name</t>
   </si>
@@ -108,16 +108,10 @@
     <t>PMA-3</t>
   </si>
   <si>
-    <t>Columbus</t>
-  </si>
-  <si>
     <t>JEM-PM / Kibo</t>
   </si>
   <si>
     <t>BEAM</t>
-  </si>
-  <si>
-    <t>Leonardo</t>
   </si>
   <si>
     <t>Nanoracks Bishop Airlock</t>
@@ -197,6 +191,30 @@
   </si>
   <si>
     <t>Active CBM magnet polarities are not consistent on Node 2 STEM Mimic model</t>
+  </si>
+  <si>
+    <t>PMM / Leonardo</t>
+  </si>
+  <si>
+    <t>COF /Columbus</t>
+  </si>
+  <si>
+    <t>COF / Columbus</t>
+  </si>
+  <si>
+    <t>MRM-1 / Rassvet</t>
+  </si>
+  <si>
+    <t>Zvezda SM</t>
+  </si>
+  <si>
+    <t>MRM-2 / Poisk</t>
+  </si>
+  <si>
+    <t>MLM / Nauka</t>
+  </si>
+  <si>
+    <t>Forward (?)</t>
   </si>
 </sst>
 </file>
@@ -581,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DC2691-CD3D-4DE6-8D5F-113A005D7514}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,13 +626,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>1</v>
@@ -623,7 +641,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -803,7 +821,7 @@
         <v>22</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -839,7 +857,7 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -872,7 +890,7 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -890,7 +908,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -908,7 +926,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -959,7 +977,7 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -977,10 +995,10 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1017,7 +1035,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>9</v>
@@ -1035,7 +1053,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>7</v>
@@ -1053,64 +1071,64 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>6</v>
@@ -1126,7 +1144,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>5</v>
@@ -1144,7 +1162,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>3</v>
@@ -1165,7 +1183,7 @@
         <v>15</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>20</v>
@@ -1179,13 +1197,13 @@
         <v>15</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1193,13 +1211,13 @@
         <v>22</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F35" t="s">
         <v>21</v>
@@ -1210,16 +1228,16 @@
         <v>22</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="F36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1227,7 +1245,7 @@
         <v>23</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>20</v>
@@ -1239,7 +1257,7 @@
         <v>21</v>
       </c>
       <c r="G37" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1247,24 +1265,24 @@
         <v>23</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="F38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F39" t="s">
         <v>22</v>
@@ -1272,18 +1290,18 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F41" t="s">
         <v>23</v>
@@ -1291,15 +1309,135 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="F47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>